<commit_message>
Added Notebook 6 and python scrapper
</commit_message>
<xml_diff>
--- a/data/extras.xlsx
+++ b/data/extras.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phoitack/Dropbox/Research/DataScience/Springboard/Mini_Projects/MEC_3.5.2_Capstone_submission/git/Springboard_MEC_3.5.2_Capstone_submission/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CD1176-2CE2-9546-B4DE-145AF0D73A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202465B6-91D7-9445-A9CB-374F3B69A77F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30500" yWindow="5600" windowWidth="27640" windowHeight="16940" xr2:uid="{343F40DA-DF0A-EC43-AB8C-F0AD61E5CA65}"/>
+    <workbookView xWindow="31200" yWindow="2340" windowWidth="30440" windowHeight="18640" xr2:uid="{343F40DA-DF0A-EC43-AB8C-F0AD61E5CA65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Spectre¬†(2015)</t>
   </si>
@@ -88,6 +88,27 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Wonder Woman</t>
+  </si>
+  <si>
+    <t>Inception</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt1375666/</t>
+  </si>
+  <si>
+    <t>Action Adventure Sci-Fi</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>https://www.imdb.com/title/tt0451279/</t>
+  </si>
+  <si>
+    <t>Action Adventure Fantasy</t>
   </si>
 </sst>
 </file>
@@ -98,10 +119,18 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,15 +153,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,16 +478,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C760197-64C0-B040-9C18-28028AD053EC}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E11"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -539,7 +574,92 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D3">
+        <v>74</v>
+      </c>
+      <c r="E3">
+        <v>148</v>
+      </c>
+      <c r="F3" s="1">
+        <v>160000000</v>
+      </c>
+      <c r="G3">
+        <v>62785337</v>
+      </c>
+      <c r="H3">
+        <v>292576195</v>
+      </c>
+      <c r="I3">
+        <v>836836967</v>
+      </c>
+      <c r="J3" s="4">
+        <v>40375</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>7.4</v>
+      </c>
+      <c r="D4">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>141</v>
+      </c>
+      <c r="F4" s="1">
+        <v>149000000</v>
+      </c>
+      <c r="G4">
+        <v>103251471</v>
+      </c>
+      <c r="H4">
+        <v>412563408</v>
+      </c>
+      <c r="I4">
+        <v>821847012</v>
+      </c>
+      <c r="J4" s="4">
+        <v>42888</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{2E12A3FA-3F63-0142-9322-2F588DAA9CE3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>